<commit_message>
Add employee rename functionality - Telegram bot commands and terminal scripts for renaming employees in Excel files
</commit_message>
<xml_diff>
--- a/Alseit.xlsx
+++ b/Alseit.xlsx
@@ -1432,7 +1432,7 @@
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr">
         <is>
-          <t>manager_7</t>
+          <t>Алихан</t>
         </is>
       </c>
       <c r="L19" t="n">
@@ -1694,7 +1694,7 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>manager_7</t>
+          <t>Алихан</t>
         </is>
       </c>
     </row>
@@ -2800,7 +2800,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>manager_7</t>
+          <t>Алихан</t>
         </is>
       </c>
       <c r="B13" t="n">

</xml_diff>